<commit_message>
tema 2+ tema 3
</commit_message>
<xml_diff>
--- a/Excel files for tables/table data Tokens.xlsx
+++ b/Excel files for tables/table data Tokens.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\Programare_TEST_folder\INTERNSHIP aquasoft\Tema2-aquasoft\Excel files for tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2D0359A-CE33-49DD-8861-25B4C6E08DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89747FE4-1490-4990-9B5E-1348E515ABF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="14430" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="14430" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table data Tokens" sheetId="1" r:id="rId1"/>
@@ -881,7 +881,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -896,7 +896,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -904,7 +904,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -912,7 +912,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -920,7 +920,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>

</xml_diff>